<commit_message>
Change format of message
</commit_message>
<xml_diff>
--- a/data/ChoiceEngineGraph.xlsx
+++ b/data/ChoiceEngineGraph.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="979" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Posts" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="71">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -41,37 +41,31 @@
     <t xml:space="preserve">Importance</t>
   </si>
   <si>
-    <t xml:space="preserve">Readme</t>
-  </si>
-  <si>
     <t xml:space="preserve">README</t>
   </si>
   <si>
-    <t xml:space="preserve">In a dark wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You are in a dark wood</t>
+    <t xml:space="preserve">About the Choice Engine project</t>
   </si>
   <si>
     <t xml:space="preserve">dark-wood</t>
   </si>
   <si>
+    <t xml:space="preserve">This is the dilemma: Things happen for a reason, but surely we are not mere things!</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">You have a map</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A map for complex territory</t>
-  </si>
-  <si>
     <t xml:space="preserve">have-map</t>
   </si>
   <si>
+    <t xml:space="preserve">Choice Engine is about the neuroscience of free will, about our intutions about freedom and choice, and about complex systems and what they can teach us about the first two things.</t>
+  </si>
+  <si>
     <t xml:space="preserve">philosophers</t>
   </si>
   <si>
-    <t xml:space="preserve">Compatiblists vs incompatibilists</t>
+    <t xml:space="preserve">You can categorise philosophers of freewill into ‘compatibalists’ and ‘incompatibalists’, based on whether they think a deterministic universe is compatible, or not, with a meaningful notion of freewill.</t>
   </si>
   <si>
     <t xml:space="preserve">high</t>
@@ -80,34 +74,25 @@
     <t xml:space="preserve">useless</t>
   </si>
   <si>
-    <t xml:space="preserve">Useless philosophy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sphex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wasp behaviour</t>
+    <t xml:space="preserve">The uselessness of philosophy</t>
   </si>
   <si>
     <t xml:space="preserve">sphexishness</t>
   </si>
   <si>
+    <t xml:space="preserve">What a wasp can help us overcome our fear of determinism</t>
+  </si>
+  <si>
     <t xml:space="preserve">determinism</t>
   </si>
   <si>
-    <t xml:space="preserve">Calvinism but no Hobbes</t>
+    <t xml:space="preserve">How people imagine determinism</t>
   </si>
   <si>
     <t xml:space="preserve">libet1</t>
   </si>
   <si>
-    <t xml:space="preserve">Experiments on free will</t>
-  </si>
-  <si>
-    <t xml:space="preserve">credits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Credits</t>
+    <t xml:space="preserve">The most famous experiment on the neuroscience of free will</t>
   </si>
   <si>
     <t xml:space="preserve">complexity</t>
@@ -116,49 +101,64 @@
     <t xml:space="preserve">A black and white world of infinite possibility</t>
   </si>
   <si>
-    <t xml:space="preserve">complexity1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasons1</t>
+    <t xml:space="preserve">reasons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reasons matter</t>
   </si>
   <si>
     <t xml:space="preserve">chaos</t>
   </si>
   <si>
-    <t xml:space="preserve">principled unpredictability</t>
+    <t xml:space="preserve">Principled unpredictability</t>
   </si>
   <si>
     <t xml:space="preserve">libet2</t>
   </si>
   <si>
-    <t xml:space="preserve">this is your brain on freewill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">libets2</t>
+    <t xml:space="preserve">Libet’s experiment, and how to escape from the claimed implications</t>
   </si>
   <si>
     <t xml:space="preserve">hyped</t>
   </si>
   <si>
-    <t xml:space="preserve">our irrationality is overhyped</t>
-  </si>
-  <si>
-    <t xml:space="preserve">truth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Truth wins</t>
+    <t xml:space="preserve">Our irrationality is overhyped</t>
   </si>
   <si>
     <t xml:space="preserve">close</t>
   </si>
   <si>
-    <t xml:space="preserve">At the heart of the wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">libert2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escape from Libet</t>
+    <t xml:space="preserve">Your choices are free because they are yours, not because they are independent of you or other structures in the world.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colophon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How we made this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intuitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our intuitions about the mind, self and world are contradictory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">causation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Causation is not the same as responsibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What happens when you tell people they aren’t free?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Want to know more?</t>
   </si>
   <si>
     <t xml:space="preserve">PostTitle</t>
@@ -170,9 +170,36 @@
     <t xml:space="preserve">LinkDestination</t>
   </si>
   <si>
+    <t xml:space="preserve">EXPTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLOSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRAIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REASONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREDITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">READING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">TAKE MAP</t>
   </si>
   <si>
+    <t xml:space="preserve">PAGE 72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAUSATION</t>
+  </si>
+  <si>
     <t xml:space="preserve">PHILOSOPHERS</t>
   </si>
   <si>
@@ -182,37 +209,31 @@
     <t xml:space="preserve">LIBET</t>
   </si>
   <si>
-    <t xml:space="preserve">MOAR PHILOSOPHY</t>
+    <t xml:space="preserve">LIBET-Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLOPHON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HYPED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTUITIONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RULE 30</t>
   </si>
   <si>
     <t xml:space="preserve">NEXT</t>
   </si>
   <si>
     <t xml:space="preserve">CHOOSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REASONS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAGE 72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RULE 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHAOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRAIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLOSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HYPED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUTH</t>
   </si>
 </sst>
 </file>
@@ -223,7 +244,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -246,6 +267,19 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -262,8 +296,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF66FF99"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <fgColor rgb="FF99FF66"/>
+        <bgColor rgb="FF66FF99"/>
       </patternFill>
     </fill>
     <fill>
@@ -314,16 +348,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,23 +377,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,11 +393,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,15 +417,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,7 +466,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FF99FF66"/>
       <rgbColor rgb="FFFFFF66"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -469,24 +499,24 @@
     <tabColor rgb="FF66FF99"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IW18"/>
+  <dimension ref="A1:IW20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A28:C33 B19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="17.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="2" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="131.214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="2" width="7.96428571428571"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -757,21 +787,21 @@
       <c r="IV1" s="4"/>
       <c r="IW1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -779,209 +809,255 @@
         <v>9</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="C6" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="C12" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+    <row r="13" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B16" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="C16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C19" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="27.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C20" s="7" t="s">
         <v>44</v>
       </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1000,23 +1076,23 @@
     <tabColor rgb="FFFFFF66"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="A28" activeCellId="0" sqref="A28:C33"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="254" min="4" style="9" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="255" style="10" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="9" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="254" min="4" style="9" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="255" style="10" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1031,332 +1107,447 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="C2" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C3" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
+      <c r="C23" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
+      <c r="B32" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
+      <c r="B33" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="16" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="16" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
+      <c r="C37" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:C1 C2:C20 C22:C33" type="list">
-      <formula1>Posts!$C$2:$C$29</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1:C3 C4:C23 C26:C35 C37:C44" type="list">
+      <formula1>Posts!$C$2:$C$28</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A20 A22:A33" type="list">
-      <formula1>Posts!$A$2:$A$29</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A4:A23 A27:A44" type="list">
+      <formula1>Posts!$A$2:$A$28</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B20 B22:B33" type="none">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4:B23 B27:B44" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>